<commit_message>
further experiments + visuals
</commit_message>
<xml_diff>
--- a/tests/adaptive400/rain2_09995_lin150k.xlsx
+++ b/tests/adaptive400/rain2_09995_lin150k.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robrecht\IdeaProjects\thesis\tests\adaptive400\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD5DE66-8904-4E9E-9E37-7E6E87341956}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59A717D-30EE-445B-B57E-6777169D4EED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="20376" windowHeight="12216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22786,8 +22786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:ABW14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="T14" sqref="T14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="A10:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -39327,6 +39327,34 @@
         <v>0.5</v>
       </c>
     </row>
+    <row r="10" spans="1:751" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f>AVERAGE(B2:NM2)</f>
+        <v>1.261780802855635</v>
+      </c>
+      <c r="B10">
+        <f>AVERAGE(NN2:ABW2)</f>
+        <v>3.0422544226260086</v>
+      </c>
+      <c r="C10">
+        <f>AVERAGE(2:2)</f>
+        <v>2.1496436479144627</v>
+      </c>
+    </row>
+    <row r="11" spans="1:751" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f>AVERAGE(B5:NM5)</f>
+        <v>0.11960392053068764</v>
+      </c>
+      <c r="B11">
+        <f>AVERAGE(NN5:ABW5)</f>
+        <v>1.340894141658086</v>
+      </c>
+      <c r="C11">
+        <f>AVERAGE(5:5)</f>
+        <v>0.72862064413288363</v>
+      </c>
+    </row>
     <row r="13" spans="1:751" x14ac:dyDescent="0.3">
       <c r="R13" t="s">
         <v>7</v>

</xml_diff>